<commit_message>
updated the related products
</commit_message>
<xml_diff>
--- a/src/data/data.xlsx
+++ b/src/data/data.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28926"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9DEF3E79-4B0B-4970-A993-A98F5DB7550B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{1835342A-A24A-4DCF-9BBC-4415276F96F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -148,7 +148,7 @@
     <t>Forjada, Templada, Revenida</t>
   </si>
   <si>
-    <t>LLAVE COROFIJA; LLAVE CORONA DOBLE ACODADA; LLAVE FIJA 1 BOCA; LLAVE TUBULAR PARA CAMIONES CON PASADOR; LLAVE SEMILUNA</t>
+    <t>LLAVE COROFIJA; LLAVE CORONA DOBLE ACODADA; LLAVE FIJA 1 BOCA; LLAVE TUBULAR PARA CAMIONES CON PASADOR</t>
   </si>
   <si>
     <t>x</t>
@@ -166,7 +166,7 @@
     <t>DIN 3113</t>
   </si>
   <si>
-    <t>LLAVE FIJA DOBLE BOCA; LLAVE CORONA DOBLE ACODADA; LLAVE FIJA 1 BOCA; LLAVE TUBULAR PARA CAMIONES CON PASADOR; LLAVE SEMILUNA</t>
+    <t>LLAVE FIJA DOBLE BOCA; LLAVE CORONA DOBLE ACODADA; LLAVE FIJA 1 BOCA; LLAVE TUBULAR PARA CAMIONES CON PASADOR</t>
   </si>
   <si>
     <t>0103</t>
@@ -196,7 +196,7 @@
     <t>DIN 838</t>
   </si>
   <si>
-    <t>LLAVE FIJA DOBLE BOCA; LLAVE COROFIJA; LLAVE FIJA 1 BOCA; LLAVE TUBULAR PARA CAMIONES CON PASADOR; LLAVE SEMILUNA</t>
+    <t>LLAVE FIJA DOBLE BOCA; LLAVE COROFIJA; LLAVE FIJA 1 BOCA; LLAVE TUBULAR PARA CAMIONES CON PASADOR</t>
   </si>
   <si>
     <t>0106</t>
@@ -217,7 +217,7 @@
     <t>DIN 894</t>
   </si>
   <si>
-    <t>LLAVE FIJA DOBLE BOCA; LLAVE COROFIJA; LLAVE CORONA DOBLE ACODADA; LLAVE TUBULAR PARA CAMIONES CON PASADOR; LLAVE SEMILUNA</t>
+    <t>LLAVE FIJA DOBLE BOCA; LLAVE COROFIJA; LLAVE CORONA DOBLE ACODADA; LLAVE TUBULAR PARA CAMIONES CON PASADOR</t>
   </si>
   <si>
     <t>0107</t>
@@ -235,7 +235,7 @@
     <t>EN 12540</t>
   </si>
   <si>
-    <t>LLAVE FIJA DOBLE BOCA; LLAVE COROFIJA; LLAVE CORONA DOBLE ACODADA; LLAVE FIJA 1 BOCA; LLAVE SEMILUNA</t>
+    <t>LLAVE FIJA DOBLE BOCA; LLAVE COROFIJA; LLAVE CORONA DOBLE ACODADA; LLAVE FIJA 1 BOCA</t>
   </si>
   <si>
     <t>0108</t>
@@ -1499,8 +1499,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:U28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
-      <selection activeCell="T14" sqref="T14"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="20.25" customHeight="1"/>

</xml_diff>